<commit_message>
Testing and introduce mean and stev fuinctions
</commit_message>
<xml_diff>
--- a/other/lab4_motion_model_data.xlsx
+++ b/other/lab4_motion_model_data.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neiman/Documents/School/CPE416/code/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2C790EB-0285-6E4E-B22A-CB9AE8634108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FB7586-FF01-4044-91B4-CB9DFFE32D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{990CA6E0-1013-CB45-B036-4CE9CC7E4520}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$G$2:$G$11</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$G$2:$G$11</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Dist</t>
   </si>
@@ -52,6 +56,15 @@
   </si>
   <si>
     <t>Ticks per In</t>
+  </si>
+  <si>
+    <t>Degrees per Inch</t>
+  </si>
+  <si>
+    <t>Degrees per Tick</t>
+  </si>
+  <si>
+    <t>Ticks per Degre</t>
   </si>
 </sst>
 </file>
@@ -104,6 +117,673 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.0</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{B8AEE69A-08B1-D549-87A7-C0C857D18563}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binCount val="5"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D20C2B22-1C56-A64D-8811-62D26E034A1B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6470650" y="2603500"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -403,15 +1083,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE86CEB-70DA-3442-9325-A9355001FD72}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -424,8 +1107,17 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -439,8 +1131,20 @@
         <f>C2/B2</f>
         <v>6.166666666666667</v>
       </c>
+      <c r="E2">
+        <f>360/81.7</f>
+        <v>4.406364749082007</v>
+      </c>
+      <c r="F2">
+        <f>E2/D2</f>
+        <v>0.71454563498627133</v>
+      </c>
+      <c r="G2">
+        <f>1/F2</f>
+        <v>1.3994907407407411</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -454,8 +1158,20 @@
         <f t="shared" ref="D3:D11" si="0">C3/B3</f>
         <v>6</v>
       </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E11" si="1">360/81.7</f>
+        <v>4.406364749082007</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F11" si="2">E3/D3</f>
+        <v>0.73439412484700117</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G11" si="3">1/F3</f>
+        <v>1.3616666666666668</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -469,8 +1185,20 @@
         <f t="shared" si="0"/>
         <v>5.833333333333333</v>
       </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>4.406364749082007</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>0.75537681412834412</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>1.3238425925925925</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -484,8 +1212,20 @@
         <f t="shared" si="0"/>
         <v>5.916666666666667</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>4.406364749082007</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>0.74473770407019835</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>1.3427546296296298</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -499,8 +1239,20 @@
         <f t="shared" si="0"/>
         <v>6.083333333333333</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>4.406364749082007</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>0.72433393135594637</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>1.3805787037037038</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -514,8 +1266,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>4.406364749082007</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>0.73439412484700117</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>1.3616666666666668</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -529,8 +1293,20 @@
         <f t="shared" si="0"/>
         <v>5.916666666666667</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>4.406364749082007</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>0.74473770407019835</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>1.3427546296296298</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -544,8 +1320,20 @@
         <f t="shared" si="0"/>
         <v>5.833333333333333</v>
       </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>4.406364749082007</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>0.75537681412834412</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>1.3238425925925925</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -559,8 +1347,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>4.406364749082007</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>0.73439412484700117</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>1.3616666666666668</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -574,8 +1374,20 @@
         <f t="shared" si="0"/>
         <v>5.833333333333333</v>
       </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>4.406364749082007</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>0.75537681412834412</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>1.3238425925925925</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -587,8 +1399,16 @@
         <f>AVERAGE(D2:D11)</f>
         <v>5.9583333333333339</v>
       </c>
+      <c r="F13">
+        <f t="shared" ref="E13:F13" si="4">AVERAGE(F2:F11)</f>
+        <v>0.73976677914086497</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13" si="5">AVERAGE(G2:G11)</f>
+        <v>1.3522106481481484</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -600,8 +1420,18 @@
         <f>STDEV(D2:D11)</f>
         <v>0.11283386673105511</v>
       </c>
+      <c r="F14">
+        <f t="shared" ref="E14:F14" si="6">STDEV(F2:F11)</f>
+        <v>1.3909688517722237E-2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14" si="7">STDEV(G2:G11)</f>
+        <v>2.5607019199797885E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>